<commit_message>
added a column for input shape
</commit_message>
<xml_diff>
--- a/models-keypoints.xlsx
+++ b/models-keypoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominika/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominika/Library/CloudStorage/OneDrive-UniversityofLeeds/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AB7520B-819A-CE48-AB2D-B9B90B84A9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BDBC65-C859-8F42-8F86-5602C2CA02C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="5060" windowWidth="26780" windowHeight="16940" xr2:uid="{1B0D5C52-EC28-504B-82BB-4D697B131FA2}"/>
+    <workbookView xWindow="380" yWindow="1060" windowWidth="26780" windowHeight="16940" xr2:uid="{1B0D5C52-EC28-504B-82BB-4D697B131FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -57,12 +57,18 @@
   </si>
   <si>
     <t>epochs</t>
+  </si>
+  <si>
+    <t>input shape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,8 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,15 +416,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716DD8F1-517E-834D-909E-B26119B5ADB6}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,74 +449,50 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D2">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="E2">
-        <v>0.126</v>
-      </c>
-      <c r="F2">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G2">
-        <v>0.59699999999999998</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.64840929210186E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9.4137497246265397E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.12839040160179099</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8.0886287614703092E-3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.58377587795257502</v>
+      </c>
+      <c r="H2" s="2">
+        <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D3">
-        <v>0.92</v>
-      </c>
-      <c r="E3">
-        <v>0.13</v>
-      </c>
-      <c r="F3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G3">
-        <v>0.60099999999999998</v>
+        <v>9</v>
+      </c>
+      <c r="H3" s="2">
+        <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D4">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="E4">
-        <v>0.127</v>
-      </c>
-      <c r="F4">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G4">
-        <v>0.59099999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
used leaky relu activation, added eval metrics
</commit_message>
<xml_diff>
--- a/models-keypoints.xlsx
+++ b/models-keypoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominika/Library/CloudStorage/OneDrive-UniversityofLeeds/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB849190-7257-664C-B1BC-22B75B46E703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9850E9-1693-104F-B63A-21514E0603BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27160" windowHeight="10720" xr2:uid="{1B0D5C52-EC28-504B-82BB-4D697B131FA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +50,6 @@
     <t>rmse</t>
   </si>
   <si>
-    <t>msle</t>
-  </si>
-  <si>
     <t>r2</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>4 + 6</t>
   </si>
   <si>
-    <t>YES YES YES</t>
-  </si>
-  <si>
     <t>extras</t>
   </si>
   <si>
@@ -116,7 +110,19 @@
     <t>input shape 300</t>
   </si>
   <si>
-    <t>augmentation</t>
+    <t>used leaky relu</t>
+  </si>
+  <si>
+    <t>yes!</t>
+  </si>
+  <si>
+    <t>looks awesome</t>
+  </si>
+  <si>
+    <t>med.</t>
+  </si>
+  <si>
+    <t>pck</t>
   </si>
 </sst>
 </file>
@@ -180,15 +186,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -507,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716DD8F1-517E-834D-909E-B26119B5ADB6}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,376 +522,484 @@
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="8">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3">
         <v>1.64840929210186E-2</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="3">
         <v>9.4137497246265397E-2</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="3">
         <v>0.12839040160179099</v>
       </c>
-      <c r="I2" s="8">
-        <v>8.0886287614703092E-3</v>
-      </c>
-      <c r="J2" s="8">
+      <c r="I2" s="3">
         <v>0.58377587795257502</v>
       </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="8">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3">
         <v>2.4206563830375599E-2</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="3">
         <v>0.114535726606845</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="3">
         <v>0.15558458864688801</v>
       </c>
-      <c r="I3" s="8">
-        <v>1.08861168846488E-2</v>
-      </c>
-      <c r="J3" s="8">
+      <c r="I3" s="3">
         <v>0.55535584688186601</v>
       </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="8">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3">
         <v>1.6472710296511602E-2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="3">
         <v>9.3701839447021401E-2</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="3">
         <v>0.12834604084491699</v>
       </c>
-      <c r="I4" s="8">
-        <v>8.1261619925498893E-3</v>
-      </c>
-      <c r="J4" s="8">
+      <c r="I4" s="3">
         <v>0.58505296707153298</v>
       </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>32</v>
-      </c>
-      <c r="C5" s="7">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>10</v>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="9">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4">
         <v>1.5914570540189701E-2</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="4">
         <v>9.1349765658378601E-2</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="4">
         <v>0.12615296244621199</v>
       </c>
-      <c r="I5" s="9">
-        <v>7.7751749195158404E-3</v>
-      </c>
-      <c r="J5" s="9">
+      <c r="I5" s="4">
         <v>0.59983921051025302</v>
       </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>16</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="8">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3">
         <v>1.7165476456284499E-2</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="3">
         <v>9.5689699053764302E-2</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="3">
         <v>0.13101710379123599</v>
       </c>
-      <c r="I6" s="8">
-        <v>8.4065543487668003E-3</v>
-      </c>
-      <c r="J6" s="8">
+      <c r="I6" s="3">
         <v>0.56695693731307895</v>
       </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>32</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>64</v>
       </c>
       <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.9595276564359599E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.10419874638319</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.13998313248157501</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.50542551279067904</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1.9595276564359599E-2</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0.10419874638319</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0.13998313248157501</v>
-      </c>
-      <c r="I7" s="8">
-        <v>9.5271794125437702E-3</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0.50542551279067904</v>
-      </c>
-      <c r="K7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6">
-        <v>32</v>
-      </c>
-      <c r="C8" s="7">
-        <v>32</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4">
         <v>5.2279159426689096E-3</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="4">
         <v>4.4275607913732501E-2</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="4">
         <v>7.2304330766201005E-2</v>
       </c>
-      <c r="I8" s="9">
-        <v>2.5057320017367601E-3</v>
-      </c>
-      <c r="J8" s="9">
+      <c r="I8" s="4">
         <v>0.86991876363754195</v>
       </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>32</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="8">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3">
         <v>1.9507434219121898E-2</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="3">
         <v>0.108136676251888</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="3">
         <v>0.13966901600360801</v>
       </c>
-      <c r="I9" s="8">
-        <v>9.5348879694938608E-3</v>
-      </c>
-      <c r="J9" s="8">
+      <c r="I9" s="3">
         <v>0.50886344909667902</v>
       </c>
-      <c r="K9" t="s">
+      <c r="J9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4">
-        <v>32</v>
-      </c>
-      <c r="C10" s="5">
-        <v>32</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5">
         <v>4.9372026696801099E-3</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="5">
         <v>4.0683008730411502E-2</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="5">
         <v>7.0265226066112504E-2</v>
       </c>
-      <c r="I10" s="10">
-        <v>2.3587024770676999E-3</v>
-      </c>
-      <c r="J10" s="10">
+      <c r="I10" s="5">
         <v>0.87691122293472201</v>
       </c>
-      <c r="K10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
         <v>23</v>
       </c>
-      <c r="C11" s="1">
-        <v>23</v>
-      </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3.91188077628612E-3</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3.4827344119548798E-2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6.2545023858547197E-2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.90296381711959794</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
         <v>26</v>
       </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
added a new iteration
</commit_message>
<xml_diff>
--- a/models-keypoints.xlsx
+++ b/models-keypoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominika/Library/CloudStorage/OneDrive-UniversityofLeeds/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9850E9-1693-104F-B63A-21514E0603BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDF65A2-673C-B04D-9FCE-3D6A980B2057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27160" windowHeight="10720" xr2:uid="{1B0D5C52-EC28-504B-82BB-4D697B131FA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -62,9 +62,6 @@
     <t>comments</t>
   </si>
   <si>
-    <t>literally the worst</t>
-  </si>
-  <si>
     <t>3 + 1</t>
   </si>
   <si>
@@ -74,30 +71,9 @@
     <t>layers (conv + dense)</t>
   </si>
   <si>
-    <t>soooo much better</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>no real improvement</t>
-  </si>
-  <si>
-    <t>ok scores</t>
-  </si>
-  <si>
-    <t>best so far</t>
-  </si>
-  <si>
-    <t>nah</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>terrible</t>
-  </si>
-  <si>
     <t>4 + 6</t>
   </si>
   <si>
@@ -113,16 +89,13 @@
     <t>used leaky relu</t>
   </si>
   <si>
-    <t>yes!</t>
-  </si>
-  <si>
-    <t>looks awesome</t>
-  </si>
-  <si>
     <t>med.</t>
   </si>
   <si>
     <t>pck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;3 </t>
   </si>
 </sst>
 </file>
@@ -159,18 +132,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -186,13 +153,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716DD8F1-517E-834D-909E-B26119B5ADB6}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,7 +493,7 @@
     <col min="10" max="11" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,10 +504,10 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -556,16 +522,16 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -576,34 +542,33 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
         <v>1.64840929210186E-2</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>9.4137497246265397E-2</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>0.12839040160179099</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>0.58377587795257502</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -614,34 +579,31 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="3">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2">
         <v>2.4206563830375599E-2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>0.114535726606845</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>0.15558458864688801</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>0.55535584688186601</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -652,34 +614,31 @@
         <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2">
         <v>1.6472710296511602E-2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>9.3701839447021401E-2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>0.12834604084491699</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>0.58505296707153298</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -690,34 +649,31 @@
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="4">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3">
         <v>1.5914570540189701E-2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>9.1349765658378601E-2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>0.12615296244621199</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>0.59983921051025302</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -728,34 +684,31 @@
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2">
         <v>1.7165476456284499E-2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>9.5689699053764302E-2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>0.13101710379123599</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>0.56695693731307895</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -766,34 +719,31 @@
         <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="3">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2">
         <v>1.9595276564359599E-2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>0.10419874638319</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>0.13998313248157501</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>0.50542551279067904</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -804,34 +754,31 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="4">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3">
         <v>5.2279159426689096E-3</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>4.4275607913732501E-2</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>7.2304330766201005E-2</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>0.86991876363754195</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -842,72 +789,66 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="3">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2">
         <v>1.9507434219121898E-2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>0.108136676251888</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>0.13966901600360801</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>0.50886344909667902</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="B10" s="4">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3">
         <v>4.9372026696801099E-3</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>4.0683008730411502E-2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>7.0265226066112504E-2</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="3">
         <v>0.87691122293472201</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -918,88 +859,88 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="3">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2">
         <v>3.91188077628612E-3</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>3.4827344119548798E-2</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>6.2545023858547197E-2</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>0.90296381711959794</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>18</v>
+      <c r="J11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="L11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>